<commit_message>
the remove_xml_specials was blocking the ISO-8859-1 special characters e.g.
&#181; = micro

corrected.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>in create_word_xml, if the path arguments don't end with "/" then it fails. This is a bit flakey…</t>
+  </si>
+  <si>
+    <t>add a function to automate building a directory structure</t>
+  </si>
+  <si>
+    <t>take the remove_rows_cols functino from RIVAS - adds in options to just do rows or just do cols</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +586,28 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43384</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43384</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added documentation for meta_table. Needs a checker/cleaner function really.
made basic test work again.. Need to do source test.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>take the remove_rows_cols functino from RIVAS - adds in options to just do rows or just do cols</t>
+  </si>
+  <si>
+    <t>remove srce() function ??</t>
+  </si>
+  <si>
+    <t>remove or revised sumby_ae ()</t>
   </si>
 </sst>
 </file>
@@ -108,12 +114,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,10 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,17 +432,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C25" sqref="C25:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.140625" customWidth="1"/>
+    <col min="3" max="3" width="176.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -475,8 +495,11 @@
       <c r="B4" s="1">
         <v>43263</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43399</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -486,12 +509,12 @@
       <c r="B5" s="1">
         <v>43263</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -502,7 +525,7 @@
       <c r="B8" s="1">
         <v>43263</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -552,6 +575,9 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
+      <c r="D12" s="1">
+        <v>43391</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -571,8 +597,11 @@
       <c r="B15" s="1">
         <v>43378</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43399</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,6 +635,28 @@
       </c>
       <c r="C20" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43399</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43399</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made attach/detach pop deal withe failures better
added in a clean_meta_table function

need to make the xlst ignore blank populations, like blank substitles...
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>remove or revised sumby_ae ()</t>
+  </si>
+  <si>
+    <t>add_progrom</t>
+  </si>
+  <si>
+    <t>attach_pop</t>
+  </si>
+  <si>
+    <t>create_word_xml</t>
+  </si>
+  <si>
+    <t>get_file_name</t>
+  </si>
+  <si>
+    <t>need to make the xls file ignore populations if they are blank.</t>
   </si>
 </sst>
 </file>
@@ -114,24 +129,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,12 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D27"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,13 +511,19 @@
       <c r="B5" s="1">
         <v>43263</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="1">
+        <v>43402</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43402</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -528,6 +536,9 @@
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D8" s="1">
+        <v>43402</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -538,6 +549,9 @@
       </c>
       <c r="C9" t="s">
         <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43402</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,6 +671,37 @@
       </c>
       <c r="C22" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43402</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made the create_word_xml work with or without the trailing slashes in filepaths
made Populations: optional in teh xslt file.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,8 +628,11 @@
       <c r="C16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -640,7 +643,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -651,7 +654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -662,7 +665,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -673,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -683,23 +686,26 @@
       <c r="C23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
fixed testing using source(). Use Local=true
used do.call rather than eval in source()..

Next is a proper vignette, testing of sumby
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -101,19 +101,13 @@
     <t>remove or revised sumby_ae ()</t>
   </si>
   <si>
-    <t>add_progrom</t>
-  </si>
-  <si>
-    <t>attach_pop</t>
-  </si>
-  <si>
-    <t>create_word_xml</t>
-  </si>
-  <si>
-    <t>get_file_name</t>
-  </si>
-  <si>
     <t>need to make the xls file ignore populations if they are blank.</t>
+  </si>
+  <si>
+    <t>Write Vignette with nested source() calls, and create code_tree figure</t>
+  </si>
+  <si>
+    <t>Testing of sumby</t>
   </si>
 </sst>
 </file>
@@ -434,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +678,7 @@
         <v>43402</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1">
         <v>43405</v>
@@ -692,22 +686,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basic test of sumby
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Testing of sumby</t>
+  </si>
+  <si>
+    <t>Not clear how to change the root calling programme name from the default of "main.R", when needed.</t>
+  </si>
+  <si>
+    <t>14/11/18 can't recreate this bug</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +603,9 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -684,14 +693,31 @@
         <v>43405</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1">
+        <v>43411</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>27</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
half way throuhg a vignette..
worked out how to do the sourcing in markdown..
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -129,12 +129,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,11 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +444,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +568,7 @@
       <c r="B10" s="1">
         <v>43263</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tweaking the vignette template.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>14/11/18 can't recreate this bug</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make the create_word_xml work in unix/mac - it uses command line ot copy files. </t>
+  </si>
+  <si>
+    <t>maybe move RESERVED to .reserved, which would be ignored in ls(), and might be cleaner? Or should I make it totally visiable..</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +727,9 @@
       <c r="C26" t="s">
         <v>26</v>
       </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -725,6 +737,16 @@
       </c>
       <c r="D27" s="1">
         <v>43418</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created an initialise which _may_ work with vignetter building...
removed some dependencies on command line
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>maybe move RESERVED to .reserved, which would be ignored in ls(), and might be cleaner? Or should I make it totally visiable..</t>
+  </si>
+  <si>
+    <t>code_tree is wrong when created in the vignette with the template/source thing.</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +746,18 @@
       <c r="C29" t="s">
         <v>31</v>
       </c>
+      <c r="D29" s="1">
+        <v>43425</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sumby, another tweak - filepaths on remote OS grrr.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -462,7 +462,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,12 +769,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
use grid.draw() in write_ggplot() which fixes background problem when using grob objects joined together.
sumby now has options to clean the text

attach_pop can call rm_envir. Closes #13

fixed an oversight in the vignette, using get_meta_table() rather than the package example meta_table data frame.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\STATISTICS\NON STUDY FOLDER\Software\R\R Code Library\cctu\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -141,12 +141,21 @@
   </si>
   <si>
     <t>reject</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>sumfig not works for ordered factor. Ordered factor class returns "ordered" "factor", fails in class checking. Suggestion: change variable.class == "factor" to any(variable.class == "factor")</t>
+  </si>
+  <si>
+    <t>SUGGESTION. sumby generates figure even set fig=F, it would be better sumby skip sumfig if fig set to F.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +808,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>34</v>
       </c>
@@ -807,7 +816,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>35</v>
       </c>
@@ -815,10 +824,31 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43480</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
       <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="1">
+        <v>43480</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vignettes not building.. tweaked how create_word_xml finds filepaths
minor bugs for sumfig/sumby
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -116,9 +116,6 @@
     <t>14/11/18 can't recreate this bug</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t xml:space="preserve">make the create_word_xml work in unix/mac - it uses command line ot copy files. </t>
   </si>
   <si>
@@ -135,9 +132,6 @@
   </si>
   <si>
     <t>issue</t>
-  </si>
-  <si>
-    <t>iSSUE</t>
   </si>
   <si>
     <t>reject</t>
@@ -479,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -608,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,8 +685,8 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="D19" t="s">
-        <v>30</v>
+      <c r="D19" s="1">
+        <v>43496</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,8 +699,8 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
-        <v>37</v>
+      <c r="D20" s="1">
+        <v>43496</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -720,7 +714,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,7 +728,7 @@
         <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +756,7 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -772,8 +766,8 @@
       <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
-        <v>30</v>
+      <c r="D26" s="1">
+        <v>43496</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,7 +780,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1">
         <v>43425</v>
@@ -794,7 +788,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="1">
         <v>43434</v>
@@ -802,7 +796,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1">
         <v>43434</v>
@@ -810,7 +804,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="1">
         <v>43434</v>
@@ -818,7 +812,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="1">
         <v>43434</v>
@@ -826,25 +820,30 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
         <v>43480</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="D35" s="1">
+        <v>43496</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <v>43480</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="D36" s="1">
+        <v>43496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #15.  Also fixed a bug with sumby and ordered factors..
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -144,16 +144,41 @@
   </si>
   <si>
     <t>sumfig doesn't work for ordered factor. Ordered factor class returns "ordered" "factor", fails in class checking. Suggestion: change variable.class == "factor" to any(variable.class == "factor")</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Installation error, "index.html": No such file or directory. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solved by deleting build folder in tar package.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sumby doesn't work for ordered factor. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -471,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,6 +871,34 @@
         <v>43496</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1">
+        <v>43496</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1">
+        <v>43497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43497</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="1">
+        <v>43497</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
closes #18 . Also more coverage in meta_table_functions.R
Made some attempts with local-repository. Not sure it works. .
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t xml:space="preserve">Sumby doesn't work for ordered factor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversion of sumby labels to propercase(?) is inconvenient for units and acronyms </t>
+  </si>
+  <si>
+    <t>there is an argument "text_clean" to override</t>
   </si>
 </sst>
 </file>
@@ -496,9 +502,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -899,6 +905,20 @@
         <v>43497</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1">
+        <v>43600</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
made create_word_xml use relative figure paths.
Closes #19  by copying the Output folder when the vignettes are built. And using devtools::build on the tar.gz fiel to build the binary.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>there is an argument "text_clean" to override</t>
+  </si>
+  <si>
+    <t>confusion caused by the meta_table object in the cctu library, versus the local users object which might be called meta_table</t>
+  </si>
+  <si>
+    <t>make it easier to get at the cctu:::cctu_env$code_tree object, or at least document it better</t>
   </si>
 </sst>
 </file>
@@ -502,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,6 +925,28 @@
         <v>43</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1">
+        <v>43664</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1">
+        <v>43664</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding in write_text(),  change the data meta_table to meta_table_example. added in get_code_tree
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>make it easier to get at the cctu:::cctu_env$code_tree object, or at least document it better</t>
+  </si>
+  <si>
+    <t>Option in write_ggplot to include survival plot from ggsurvplot - package survminer</t>
+  </si>
+  <si>
+    <t>JK</t>
+  </si>
+  <si>
+    <t>Now it is meta_table_example</t>
+  </si>
+  <si>
+    <t>added a get_code_tree() function and improved the help page</t>
   </si>
 </sst>
 </file>
@@ -508,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +851,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>33</v>
       </c>
@@ -847,7 +859,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>34</v>
       </c>
@@ -855,7 +867,7 @@
         <v>43434</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -869,7 +881,7 @@
         <v>43496</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -883,7 +895,7 @@
         <v>43496</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -897,7 +909,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -911,7 +923,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -925,7 +937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -935,8 +947,14 @@
       <c r="C41" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <v>43724</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -945,6 +963,23 @@
       </c>
       <c r="C42" t="s">
         <v>45</v>
+      </c>
+      <c r="D42" s="1">
+        <v>43724</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1">
+        <v>43713</v>
+      </c>
+      <c r="C43" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improving testing. Added in a warning when calling source() without using cctu_initialise.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -187,12 +187,15 @@
   <si>
     <t>added a get_code_tree() function and improved the help page</t>
   </si>
+  <si>
+    <t>In Rivas, calling the configuration file created an error somewhere. This was solved by running cctu_initialise.  Produce a helpful error message or automate the call?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +210,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +231,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -231,17 +246,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,6 +1000,20 @@
         <v>46</v>
       </c>
     </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1">
+        <v>43752</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="1">
+        <v>43752</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
checking of code-tree existing in source was failling always - code error now fixed
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11820"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -190,12 +190,18 @@
   <si>
     <t>In Rivas, calling the configuration file created an error somewhere. This was solved by running cctu_initialise.  Produce a helpful error message or automate the call?</t>
   </si>
+  <si>
+    <t>If sumby is fed an empty or all NA variable, then the sumfig crashes. Add a check in and disable the figure.</t>
+  </si>
+  <si>
+    <t>Give a better warning if .reserved is undefined in clean_up()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,8 +223,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +249,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -246,19 +264,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -538,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,6 +1035,28 @@
         <v>43752</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1">
+        <v>43754</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="1">
+        <v>43754</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding in read_data and data_table_summary
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Give a better warning if .reserved is undefined in clean_up()</t>
+  </si>
+  <si>
+    <t>Is there a case for make a function to produce a compact frequency table for a sequence of binary variables, that just give the count/percent for yeses</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,6 +1060,14 @@
         <v>52</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>43756</v>
+      </c>
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
improving coverage, deleting spurious lines from sumby.  Making the testing in sumby write output to a tempdir()
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Is there a case for make a function to produce a compact frequency table for a sequence of binary variables, that just give the count/percent for yeses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit the rmarkdown.Rmd and add text.rmd as per Rivas, to get text.xml into the HTML report. </t>
   </si>
 </sst>
 </file>
@@ -562,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,6 +1071,14 @@
         <v>53</v>
       </c>
     </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>43769</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed some more bugs, cleaned code to get higher test coverage.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -568,7 +568,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,8 +1059,11 @@
       <c r="B47" s="1">
         <v>43754</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>52</v>
+      </c>
+      <c r="D47" s="1">
+        <v>43790</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,12 +1074,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>43769</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="5" t="s">
         <v>54</v>
+      </c>
+      <c r="D49" s="1">
+        <v>43790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a bug with sumby
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -207,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,15 +229,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,11 +248,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -270,22 +258,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -568,7 +553,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,8 +1033,11 @@
       <c r="B46" s="1">
         <v>43754</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>51</v>
+      </c>
+      <c r="D46" s="1">
+        <v>43811</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding featuer to sumby - can delete levels if desired from the frequency tables. provide a value to Delete
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t xml:space="preserve">Edit the rmarkdown.Rmd and add text.rmd as per Rivas, to get text.xml into the HTML report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">added in a "delete=" argument to remove levels if desired. </t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,8 +1061,14 @@
       <c r="B48" s="1">
         <v>43756</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="5" t="s">
         <v>53</v>
+      </c>
+      <c r="D48" s="1">
+        <v>43815</v>
+      </c>
+      <c r="E48" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated sumby so that factors with labels containing spaces are not "tidied" up
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t xml:space="preserve">added in a "delete=" argument to remove levels if desired. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">in sumby if the factor labels have spaces in then the heading in the output is "tidied". Disable this. </t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1074,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>43769</v>
       </c>
@@ -1080,6 +1083,20 @@
       </c>
       <c r="D49" s="1">
         <v>43790</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44125</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="1">
+        <v>44125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to set up github actions for CI
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>Person Raising Bug</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t xml:space="preserve">in sumby if the factor labels have spaces in then the heading in the output is "tidied". Disable this. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">if write_ggplot has format="postscript" then we want the file output to have suffix ".eps", and not ".postscript". </t>
+  </si>
+  <si>
+    <t>write_table doesn't deal with tibble data frames correctly, and converts factors to levels rather than labels - maybe just (if(inherits(data,"tibble")){data&lt;- as.data.frame(data)}</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +260,18 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -268,13 +286,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -556,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,6 +1119,25 @@
         <v>44125</v>
       </c>
     </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44131</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>44153</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bug fixes with postscript figure output, and write_table with tibble input.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -242,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,13 +262,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -579,7 +573,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,6 +1123,9 @@
       <c r="C53" s="6" t="s">
         <v>57</v>
       </c>
+      <c r="D53" s="1">
+        <v>44159</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
@@ -1136,6 +1133,9 @@
       </c>
       <c r="C54" s="7" t="s">
         <v>58</v>
+      </c>
+      <c r="D54" s="1">
+        <v>44159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>